<commit_message>
fuck it. dates will have timestamps
</commit_message>
<xml_diff>
--- a/new-init.xlsx
+++ b/new-init.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -52,10 +52,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -331,7 +332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -383,7 +384,7 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43599</v>
+        <v>43597</v>
       </c>
     </row>
     <row r="3">
@@ -393,7 +394,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43600</v>
+        <v>43598</v>
       </c>
     </row>
     <row r="4">
@@ -403,7 +404,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43601</v>
+        <v>43599</v>
       </c>
     </row>
     <row r="5">
@@ -413,7 +414,7 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43602</v>
+        <v>43600</v>
       </c>
     </row>
     <row r="6">
@@ -423,7 +424,7 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>43603</v>
+        <v>43601</v>
       </c>
     </row>
     <row r="7">
@@ -433,7 +434,7 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43604</v>
+        <v>43602</v>
       </c>
     </row>
     <row r="8">
@@ -443,7 +444,7 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43605</v>
+        <v>43603</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +500,7 @@
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>43606</v>
+        <v>43604</v>
       </c>
     </row>
     <row r="12">
@@ -509,7 +510,7 @@
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>43607</v>
+        <v>43605</v>
       </c>
     </row>
     <row r="13">
@@ -519,7 +520,7 @@
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>43608</v>
+        <v>43606</v>
       </c>
     </row>
     <row r="14">
@@ -529,7 +530,7 @@
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>43609</v>
+        <v>43607</v>
       </c>
     </row>
     <row r="15">
@@ -539,7 +540,7 @@
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>43610</v>
+        <v>43608</v>
       </c>
     </row>
     <row r="16">
@@ -549,7 +550,7 @@
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>43611</v>
+        <v>43609</v>
       </c>
     </row>
     <row r="17">
@@ -559,7 +560,7 @@
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>43612</v>
+        <v>43610</v>
       </c>
     </row>
     <row r="18">
@@ -571,6 +572,244 @@
       <c r="F18" s="2" t="n"/>
       <c r="G18" s="2" t="n"/>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>End</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>End</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>43611</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>43612</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>43615</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>43616</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0.2291666666666667</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>43617</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n"/>
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="n"/>
+      <c r="E27" s="2" t="n"/>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="2" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>End</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>End</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Sun</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>43618</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>43619</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Tue</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>43620</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>43621</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Thu</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>43622</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>43623</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Sat</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n"/>
+      <c r="B36" s="2" t="n"/>
+      <c r="C36" s="2" t="n"/>
+      <c r="D36" s="2" t="n"/>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="n"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
basic functionality works after moving sheet1 to main.py
</commit_message>
<xml_diff>
--- a/new-init.xlsx
+++ b/new-init.xlsx
@@ -52,10 +52,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2241,6 +2242,18 @@
       <c r="B146" s="1" t="n">
         <v>43709</v>
       </c>
+      <c r="C146" s="3" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="D146" s="3" t="n">
+        <v>0.08333333333333333</v>
+      </c>
+      <c r="E146" s="3" t="n">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="F146" s="3" t="n">
+        <v>0.4243055555555555</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">

</xml_diff>

<commit_message>
added tkinter tutorial for later work on gui
</commit_message>
<xml_diff>
--- a/new-init.xlsx
+++ b/new-init.xlsx
@@ -386,6 +386,12 @@
       <c r="B2" s="1" t="n">
         <v>43597</v>
       </c>
+      <c r="C2" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -396,6 +402,12 @@
       <c r="B3" s="1" t="n">
         <v>43598</v>
       </c>
+      <c r="C3" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -406,6 +418,12 @@
       <c r="B4" s="1" t="n">
         <v>43599</v>
       </c>
+      <c r="C4" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -416,6 +434,12 @@
       <c r="B5" s="1" t="n">
         <v>43600</v>
       </c>
+      <c r="C5" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -426,6 +450,12 @@
       <c r="B6" s="1" t="n">
         <v>43601</v>
       </c>
+      <c r="C6" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -436,6 +466,12 @@
       <c r="B7" s="1" t="n">
         <v>43602</v>
       </c>
+      <c r="C7" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -445,6 +481,12 @@
       </c>
       <c r="B8" s="1" t="n">
         <v>43603</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="9">
@@ -502,6 +544,12 @@
       <c r="B11" s="1" t="n">
         <v>43604</v>
       </c>
+      <c r="C11" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -512,6 +560,12 @@
       <c r="B12" s="1" t="n">
         <v>43605</v>
       </c>
+      <c r="C12" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -522,6 +576,12 @@
       <c r="B13" s="1" t="n">
         <v>43606</v>
       </c>
+      <c r="C13" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -532,6 +592,12 @@
       <c r="B14" s="1" t="n">
         <v>43607</v>
       </c>
+      <c r="C14" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -542,6 +608,12 @@
       <c r="B15" s="1" t="n">
         <v>43608</v>
       </c>
+      <c r="C15" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -552,6 +624,12 @@
       <c r="B16" s="1" t="n">
         <v>43609</v>
       </c>
+      <c r="C16" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -561,6 +639,12 @@
       </c>
       <c r="B17" s="1" t="n">
         <v>43610</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="18">
@@ -618,6 +702,12 @@
       <c r="B20" s="1" t="n">
         <v>43611</v>
       </c>
+      <c r="C20" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -628,6 +718,12 @@
       <c r="B21" s="1" t="n">
         <v>43612</v>
       </c>
+      <c r="C21" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -638,6 +734,12 @@
       <c r="B22" s="1" t="n">
         <v>43613</v>
       </c>
+      <c r="C22" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -648,6 +750,12 @@
       <c r="B23" s="1" t="n">
         <v>43614</v>
       </c>
+      <c r="C23" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -658,6 +766,12 @@
       <c r="B24" s="1" t="n">
         <v>43615</v>
       </c>
+      <c r="C24" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -668,6 +782,12 @@
       <c r="B25" s="1" t="n">
         <v>43616</v>
       </c>
+      <c r="C25" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -677,6 +797,12 @@
       </c>
       <c r="B26" s="1" t="n">
         <v>43617</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="27">
@@ -734,6 +860,12 @@
       <c r="B29" s="1" t="n">
         <v>43618</v>
       </c>
+      <c r="C29" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -744,6 +876,12 @@
       <c r="B30" s="1" t="n">
         <v>43619</v>
       </c>
+      <c r="C30" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -754,6 +892,12 @@
       <c r="B31" s="1" t="n">
         <v>43620</v>
       </c>
+      <c r="C31" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -764,6 +908,12 @@
       <c r="B32" s="1" t="n">
         <v>43621</v>
       </c>
+      <c r="C32" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -774,6 +924,12 @@
       <c r="B33" s="1" t="n">
         <v>43622</v>
       </c>
+      <c r="C33" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -784,6 +940,12 @@
       <c r="B34" s="1" t="n">
         <v>43623</v>
       </c>
+      <c r="C34" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -793,6 +955,12 @@
       </c>
       <c r="B35" s="1" t="n">
         <v>43624</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="36">
@@ -850,6 +1018,12 @@
       <c r="B38" s="1" t="n">
         <v>43625</v>
       </c>
+      <c r="C38" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -860,6 +1034,12 @@
       <c r="B39" s="1" t="n">
         <v>43626</v>
       </c>
+      <c r="C39" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -870,6 +1050,12 @@
       <c r="B40" s="1" t="n">
         <v>43627</v>
       </c>
+      <c r="C40" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -880,6 +1066,12 @@
       <c r="B41" s="1" t="n">
         <v>43628</v>
       </c>
+      <c r="C41" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -890,6 +1082,12 @@
       <c r="B42" s="1" t="n">
         <v>43629</v>
       </c>
+      <c r="C42" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -900,6 +1098,12 @@
       <c r="B43" s="1" t="n">
         <v>43630</v>
       </c>
+      <c r="C43" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -909,6 +1113,12 @@
       </c>
       <c r="B44" s="1" t="n">
         <v>43631</v>
+      </c>
+      <c r="C44" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="45">
@@ -966,6 +1176,12 @@
       <c r="B47" s="1" t="n">
         <v>43632</v>
       </c>
+      <c r="C47" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -976,6 +1192,12 @@
       <c r="B48" s="1" t="n">
         <v>43633</v>
       </c>
+      <c r="C48" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -986,6 +1208,12 @@
       <c r="B49" s="1" t="n">
         <v>43634</v>
       </c>
+      <c r="C49" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -996,6 +1224,12 @@
       <c r="B50" s="1" t="n">
         <v>43635</v>
       </c>
+      <c r="C50" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1006,6 +1240,12 @@
       <c r="B51" s="1" t="n">
         <v>43636</v>
       </c>
+      <c r="C51" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1016,6 +1256,12 @@
       <c r="B52" s="1" t="n">
         <v>43637</v>
       </c>
+      <c r="C52" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1025,6 +1271,12 @@
       </c>
       <c r="B53" s="1" t="n">
         <v>43638</v>
+      </c>
+      <c r="C53" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="54">
@@ -1082,6 +1334,12 @@
       <c r="B56" s="1" t="n">
         <v>43639</v>
       </c>
+      <c r="C56" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1092,6 +1350,12 @@
       <c r="B57" s="1" t="n">
         <v>43640</v>
       </c>
+      <c r="C57" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1102,6 +1366,12 @@
       <c r="B58" s="1" t="n">
         <v>43641</v>
       </c>
+      <c r="C58" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1112,6 +1382,12 @@
       <c r="B59" s="1" t="n">
         <v>43642</v>
       </c>
+      <c r="C59" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1122,6 +1398,12 @@
       <c r="B60" s="1" t="n">
         <v>43643</v>
       </c>
+      <c r="C60" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1132,6 +1414,12 @@
       <c r="B61" s="1" t="n">
         <v>43644</v>
       </c>
+      <c r="C61" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1141,6 +1429,12 @@
       </c>
       <c r="B62" s="1" t="n">
         <v>43645</v>
+      </c>
+      <c r="C62" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="63">
@@ -1198,6 +1492,12 @@
       <c r="B65" s="1" t="n">
         <v>43646</v>
       </c>
+      <c r="C65" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1208,6 +1508,12 @@
       <c r="B66" s="1" t="n">
         <v>43647</v>
       </c>
+      <c r="C66" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1218,6 +1524,12 @@
       <c r="B67" s="1" t="n">
         <v>43648</v>
       </c>
+      <c r="C67" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1228,6 +1540,12 @@
       <c r="B68" s="1" t="n">
         <v>43649</v>
       </c>
+      <c r="C68" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1238,6 +1556,12 @@
       <c r="B69" s="1" t="n">
         <v>43650</v>
       </c>
+      <c r="C69" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1248,6 +1572,12 @@
       <c r="B70" s="1" t="n">
         <v>43651</v>
       </c>
+      <c r="C70" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1257,6 +1587,12 @@
       </c>
       <c r="B71" s="1" t="n">
         <v>43652</v>
+      </c>
+      <c r="C71" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="72">
@@ -1314,6 +1650,12 @@
       <c r="B74" s="1" t="n">
         <v>43653</v>
       </c>
+      <c r="C74" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1324,6 +1666,12 @@
       <c r="B75" s="1" t="n">
         <v>43654</v>
       </c>
+      <c r="C75" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1334,6 +1682,12 @@
       <c r="B76" s="1" t="n">
         <v>43655</v>
       </c>
+      <c r="C76" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>0.1979166666666667</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1343,6 +1697,12 @@
       </c>
       <c r="B77" s="1" t="n">
         <v>43656</v>
+      </c>
+      <c r="C77" s="3" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="D77" s="3" t="n">
+        <v>0.1979166666666667</v>
       </c>
     </row>
     <row r="78">
@@ -2242,18 +2602,6 @@
       <c r="B146" s="1" t="n">
         <v>43709</v>
       </c>
-      <c r="C146" s="3" t="n">
-        <v>0.04166666666666666</v>
-      </c>
-      <c r="D146" s="3" t="n">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="E146" s="3" t="n">
-        <v>0.2916666666666667</v>
-      </c>
-      <c r="F146" s="3" t="n">
-        <v>0.4243055555555555</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">

</xml_diff>